<commit_message>
added initial settings for static inputs, refclk clock outputs
</commit_message>
<xml_diff>
--- a/examples/EMTF_vu13p/src/protocol_10g.xlsx
+++ b/examples/EMTF_vu13p/src/protocol_10g.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1878" uniqueCount="1143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1876" uniqueCount="1141">
   <si>
     <t xml:space="preserve">// path</t>
   </si>
@@ -3347,12 +3347,6 @@
   </si>
   <si>
     <t xml:space="preserve">should be 4’b1010 for 800 mV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RXPD, TXPD,QPLLPD,CPLLPD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">set all of these to all 1, to have power down by default</t>
   </si>
   <si>
     <t xml:space="preserve">If RXSLIDE is used, set the following:</t>
@@ -3587,8 +3581,8 @@
   </sheetPr>
   <dimension ref="A1:D721"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A364" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A391" activeCellId="0" sqref="A391"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A508" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A524" activeCellId="1" sqref="C21:H21 A524"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10019,7 +10013,7 @@
         <v>817</v>
       </c>
       <c r="B643" s="4" t="s">
-        <v>116</v>
+        <v>460</v>
       </c>
       <c r="C643" s="4"/>
       <c r="D643" s="4"/>
@@ -10549,7 +10543,7 @@
         <v>873</v>
       </c>
       <c r="B696" s="4" t="s">
-        <v>116</v>
+        <v>460</v>
       </c>
       <c r="C696" s="4"/>
       <c r="D696" s="4"/>
@@ -10808,8 +10802,8 @@
   </sheetPr>
   <dimension ref="A1:D181"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A99" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A111" activeCellId="0" sqref="A111"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A127" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B144" activeCellId="1" sqref="C21:H21 B144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12243,7 +12237,7 @@
         <v>1042</v>
       </c>
       <c r="B143" s="4" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="C143" s="0"/>
       <c r="D143" s="0"/>
@@ -12647,7 +12641,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="1" sqref="C21:H21 B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12719,7 +12713,7 @@
   <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C26" activeCellId="0" sqref="C26"/>
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21:H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12854,16 +12848,11 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C21" s="6" t="s">
-        <v>1108</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>1109</v>
-      </c>
+      <c r="C21" s="6"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="6" t="s">
-        <v>1110</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12904,12 +12893,12 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="0" t="s">
-        <v>1111</v>
+        <v>1109</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C29" s="3" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="D29" s="0" t="s">
         <v>1098</v>
@@ -12917,133 +12906,133 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C30" s="0" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="0" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="0" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="0" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="0" t="s">
-        <v>1120</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C37" s="0" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="0" t="s">
-        <v>1122</v>
+        <v>1120</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="0" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="0" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="1" t="s">
-        <v>1127</v>
+        <v>1125</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C45" s="1" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C46" s="1" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C47" s="1" t="s">
-        <v>1133</v>
+        <v>1131</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>1134</v>
+        <v>1132</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C48" s="1" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>1136</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="1" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C50" s="1" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C51" s="1" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>1142</v>
+        <v>1140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>